<commit_message>
task 1 finished and tuned
</commit_message>
<xml_diff>
--- a/data/summed_interventions_long.xlsx
+++ b/data/summed_interventions_long.xlsx
@@ -10,6 +10,59 @@
     <sheet name="Total_Interventions" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+  <si>
+    <t xml:space="preserve">year.announced</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gta.evaluation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">count</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2009</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Green</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Red</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2010</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2011</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2012</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2013</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2014</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -338,7 +391,349 @@
     <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="n">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="n">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="n">
+        <v>1298</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="n">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" t="n">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="n">
+        <v>1132</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" t="n">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" t="n">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" t="n">
+        <v>1142</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" t="n">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" t="n">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" t="n">
+        <v>1421</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" t="n">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" t="n">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" t="n">
+        <v>1367</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" t="n">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" t="n">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>12</v>
+      </c>
+      <c r="B20" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20" t="n">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" t="n">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" t="n">
+        <v>1196</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23" t="n">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>13</v>
+      </c>
+      <c r="B24" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" t="n">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>13</v>
+      </c>
+      <c r="B25" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" t="n">
+        <v>1089</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>14</v>
+      </c>
+      <c r="B26" t="s">
+        <v>4</v>
+      </c>
+      <c r="C26" t="n">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>14</v>
+      </c>
+      <c r="B27" t="s">
+        <v>5</v>
+      </c>
+      <c r="C27" t="n">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>14</v>
+      </c>
+      <c r="B28" t="s">
+        <v>6</v>
+      </c>
+      <c r="C28" t="n">
+        <v>1201</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>15</v>
+      </c>
+      <c r="B29" t="s">
+        <v>4</v>
+      </c>
+      <c r="C29" t="n">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>15</v>
+      </c>
+      <c r="B30" t="s">
+        <v>5</v>
+      </c>
+      <c r="C30" t="n">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
+        <v>15</v>
+      </c>
+      <c r="B31" t="s">
+        <v>6</v>
+      </c>
+      <c r="C31" t="n">
+        <v>1059</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
@@ -351,7 +746,96 @@
     <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="n">
+        <v>1880</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="n">
+        <v>1728</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="n">
+        <v>1753</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="n">
+        <v>2105</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="n">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="n">
+        <v>1891</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" t="n">
+        <v>1943</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" t="n">
+        <v>1753</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" t="n">
+        <v>1809</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" t="n">
+        <v>1635</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>

</xml_diff>